<commit_message>
test RC QFT cratio
</commit_message>
<xml_diff>
--- a/comratio/cratios/QFT_10.xlsx
+++ b/comratio/cratios/QFT_10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:B66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,21 +439,6 @@
           <t>RC</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>SZ</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>ZFP</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>FPZIP</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -462,15 +447,6 @@
       <c r="B2" t="n">
         <v>0.015625</v>
       </c>
-      <c r="C2" t="n">
-        <v>0.00927734375</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.00927734375</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.00927734375</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -479,15 +455,6 @@
       <c r="B3" t="n">
         <v>0.03125</v>
       </c>
-      <c r="C3" t="n">
-        <v>0.013427734375</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.013427734375</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.013427734375</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -496,15 +463,6 @@
       <c r="B4" t="n">
         <v>0.0625</v>
       </c>
-      <c r="C4" t="n">
-        <v>0.021728515625</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.021728515625</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.021728515625</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -513,15 +471,6 @@
       <c r="B5" t="n">
         <v>0.125</v>
       </c>
-      <c r="C5" t="n">
-        <v>0.0382080078125</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.0382080078125</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.0382080078125</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -530,15 +479,6 @@
       <c r="B6" t="n">
         <v>0.25</v>
       </c>
-      <c r="C6" t="n">
-        <v>0.070556640625</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.070556640625</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.070556640625</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -547,15 +487,6 @@
       <c r="B7" t="n">
         <v>0.125</v>
       </c>
-      <c r="C7" t="n">
-        <v>0.0400390625</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.0400390625</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.0400390625</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -564,15 +495,6 @@
       <c r="B8" t="n">
         <v>0.0625</v>
       </c>
-      <c r="C8" t="n">
-        <v>0.023681640625</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.023681640625</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.023681640625</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -581,15 +503,6 @@
       <c r="B9" t="n">
         <v>0.03125</v>
       </c>
-      <c r="C9" t="n">
-        <v>0.015869140625</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.015869140625</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.015869140625</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -598,15 +511,6 @@
       <c r="B10" t="n">
         <v>0.015625</v>
       </c>
-      <c r="C10" t="n">
-        <v>0.0123291015625</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.0123291015625</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.0123291015625</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -615,15 +519,6 @@
       <c r="B11" t="n">
         <v>0.0078125</v>
       </c>
-      <c r="C11" t="n">
-        <v>0.01025390625</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.01025390625</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.01025390625</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -632,15 +527,6 @@
       <c r="B12" t="n">
         <v>0.125</v>
       </c>
-      <c r="C12" t="n">
-        <v>0.0416259765625</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0.0416259765625</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.0416259765625</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -649,15 +535,6 @@
       <c r="B13" t="n">
         <v>0.125</v>
       </c>
-      <c r="C13" t="n">
-        <v>0.04296875</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.04296875</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0.04296875</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -666,15 +543,6 @@
       <c r="B14" t="n">
         <v>0.0625</v>
       </c>
-      <c r="C14" t="n">
-        <v>0.0419921875</v>
-      </c>
-      <c r="D14" t="n">
-        <v>0.0419921875</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0.0419921875</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -683,15 +551,6 @@
       <c r="B15" t="n">
         <v>0.0625</v>
       </c>
-      <c r="C15" t="n">
-        <v>0.0416259765625</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0.0416259765625</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0.0416259765625</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -700,15 +559,6 @@
       <c r="B16" t="n">
         <v>0.0625</v>
       </c>
-      <c r="C16" t="n">
-        <v>0.041259765625</v>
-      </c>
-      <c r="D16" t="n">
-        <v>0.041259765625</v>
-      </c>
-      <c r="E16" t="n">
-        <v>0.041259765625</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -717,15 +567,6 @@
       <c r="B17" t="n">
         <v>0.03125</v>
       </c>
-      <c r="C17" t="n">
-        <v>0.0411376953125</v>
-      </c>
-      <c r="D17" t="n">
-        <v>0.0411376953125</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0.0411376953125</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -734,15 +575,6 @@
       <c r="B18" t="n">
         <v>0.03125</v>
       </c>
-      <c r="C18" t="n">
-        <v>0.0408935546875</v>
-      </c>
-      <c r="D18" t="n">
-        <v>0.0408935546875</v>
-      </c>
-      <c r="E18" t="n">
-        <v>0.0408935546875</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -751,15 +583,6 @@
       <c r="B19" t="n">
         <v>0.03125</v>
       </c>
-      <c r="C19" t="n">
-        <v>0.040771484375</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0.040771484375</v>
-      </c>
-      <c r="E19" t="n">
-        <v>0.040771484375</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -768,15 +591,6 @@
       <c r="B20" t="n">
         <v>0.03125</v>
       </c>
-      <c r="C20" t="n">
-        <v>0.04052734375</v>
-      </c>
-      <c r="D20" t="n">
-        <v>0.04052734375</v>
-      </c>
-      <c r="E20" t="n">
-        <v>0.04052734375</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -785,15 +599,6 @@
       <c r="B21" t="n">
         <v>0.015625</v>
       </c>
-      <c r="C21" t="n">
-        <v>0.0411376953125</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0.0411376953125</v>
-      </c>
-      <c r="E21" t="n">
-        <v>0.0411376953125</v>
-      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -802,15 +607,6 @@
       <c r="B22" t="n">
         <v>0.0234375</v>
       </c>
-      <c r="C22" t="n">
-        <v>0.0411376953125</v>
-      </c>
-      <c r="D22" t="n">
-        <v>0.0411376953125</v>
-      </c>
-      <c r="E22" t="n">
-        <v>0.0411376953125</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -819,15 +615,6 @@
       <c r="B23" t="n">
         <v>0.0234375</v>
       </c>
-      <c r="C23" t="n">
-        <v>0.041015625</v>
-      </c>
-      <c r="D23" t="n">
-        <v>0.041015625</v>
-      </c>
-      <c r="E23" t="n">
-        <v>0.041015625</v>
-      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -836,15 +623,6 @@
       <c r="B24" t="n">
         <v>0.0234375</v>
       </c>
-      <c r="C24" t="n">
-        <v>0.0411376953125</v>
-      </c>
-      <c r="D24" t="n">
-        <v>0.0411376953125</v>
-      </c>
-      <c r="E24" t="n">
-        <v>0.0411376953125</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -853,15 +631,6 @@
       <c r="B25" t="n">
         <v>0.0234375</v>
       </c>
-      <c r="C25" t="n">
-        <v>0.0411376953125</v>
-      </c>
-      <c r="D25" t="n">
-        <v>0.0411376953125</v>
-      </c>
-      <c r="E25" t="n">
-        <v>0.0411376953125</v>
-      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -870,15 +639,6 @@
       <c r="B26" t="n">
         <v>0.0234375</v>
       </c>
-      <c r="C26" t="n">
-        <v>0.0408935546875</v>
-      </c>
-      <c r="D26" t="n">
-        <v>0.0408935546875</v>
-      </c>
-      <c r="E26" t="n">
-        <v>0.0408935546875</v>
-      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -887,15 +647,6 @@
       <c r="B27" t="n">
         <v>0.0234375</v>
       </c>
-      <c r="C27" t="n">
-        <v>0.0408935546875</v>
-      </c>
-      <c r="D27" t="n">
-        <v>0.0408935546875</v>
-      </c>
-      <c r="E27" t="n">
-        <v>0.0408935546875</v>
-      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -904,15 +655,6 @@
       <c r="B28" t="n">
         <v>0.0234375</v>
       </c>
-      <c r="C28" t="n">
-        <v>0.041015625</v>
-      </c>
-      <c r="D28" t="n">
-        <v>0.041015625</v>
-      </c>
-      <c r="E28" t="n">
-        <v>0.041015625</v>
-      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -921,15 +663,6 @@
       <c r="B29" t="n">
         <v>0.0234375</v>
       </c>
-      <c r="C29" t="n">
-        <v>0.0408935546875</v>
-      </c>
-      <c r="D29" t="n">
-        <v>0.0408935546875</v>
-      </c>
-      <c r="E29" t="n">
-        <v>0.0408935546875</v>
-      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -938,15 +671,6 @@
       <c r="B30" t="n">
         <v>0.0234375</v>
       </c>
-      <c r="C30" t="n">
-        <v>0.0408935546875</v>
-      </c>
-      <c r="D30" t="n">
-        <v>0.0408935546875</v>
-      </c>
-      <c r="E30" t="n">
-        <v>0.0408935546875</v>
-      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -955,15 +679,6 @@
       <c r="B31" t="n">
         <v>0.0234375</v>
       </c>
-      <c r="C31" t="n">
-        <v>0.041015625</v>
-      </c>
-      <c r="D31" t="n">
-        <v>0.041015625</v>
-      </c>
-      <c r="E31" t="n">
-        <v>0.041015625</v>
-      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -972,15 +687,6 @@
       <c r="B32" t="n">
         <v>0.046875</v>
       </c>
-      <c r="C32" t="n">
-        <v>0.0784912109375</v>
-      </c>
-      <c r="D32" t="n">
-        <v>0.0784912109375</v>
-      </c>
-      <c r="E32" t="n">
-        <v>0.0784912109375</v>
-      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -989,15 +695,6 @@
       <c r="B33" t="n">
         <v>0.046875</v>
       </c>
-      <c r="C33" t="n">
-        <v>0.0784912109375</v>
-      </c>
-      <c r="D33" t="n">
-        <v>0.0784912109375</v>
-      </c>
-      <c r="E33" t="n">
-        <v>0.0784912109375</v>
-      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -1006,15 +703,6 @@
       <c r="B34" t="n">
         <v>0.046875</v>
       </c>
-      <c r="C34" t="n">
-        <v>0.0784912109375</v>
-      </c>
-      <c r="D34" t="n">
-        <v>0.0784912109375</v>
-      </c>
-      <c r="E34" t="n">
-        <v>0.0784912109375</v>
-      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -1023,15 +711,6 @@
       <c r="B35" t="n">
         <v>0.046875</v>
       </c>
-      <c r="C35" t="n">
-        <v>0.0784912109375</v>
-      </c>
-      <c r="D35" t="n">
-        <v>0.0784912109375</v>
-      </c>
-      <c r="E35" t="n">
-        <v>0.0784912109375</v>
-      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -1040,15 +719,6 @@
       <c r="B36" t="n">
         <v>0.046875</v>
       </c>
-      <c r="C36" t="n">
-        <v>0.0784912109375</v>
-      </c>
-      <c r="D36" t="n">
-        <v>0.0784912109375</v>
-      </c>
-      <c r="E36" t="n">
-        <v>0.0784912109375</v>
-      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -1057,15 +727,6 @@
       <c r="B37" t="n">
         <v>0.046875</v>
       </c>
-      <c r="C37" t="n">
-        <v>0.0784912109375</v>
-      </c>
-      <c r="D37" t="n">
-        <v>0.0784912109375</v>
-      </c>
-      <c r="E37" t="n">
-        <v>0.0784912109375</v>
-      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -1074,15 +735,6 @@
       <c r="B38" t="n">
         <v>0.046875</v>
       </c>
-      <c r="C38" t="n">
-        <v>0.0784912109375</v>
-      </c>
-      <c r="D38" t="n">
-        <v>0.0784912109375</v>
-      </c>
-      <c r="E38" t="n">
-        <v>0.0784912109375</v>
-      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -1091,15 +743,6 @@
       <c r="B39" t="n">
         <v>0.09375</v>
       </c>
-      <c r="C39" t="n">
-        <v>0.138427734375</v>
-      </c>
-      <c r="D39" t="n">
-        <v>0.138427734375</v>
-      </c>
-      <c r="E39" t="n">
-        <v>0.138427734375</v>
-      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -1108,15 +751,6 @@
       <c r="B40" t="n">
         <v>0.09375</v>
       </c>
-      <c r="C40" t="n">
-        <v>0.138427734375</v>
-      </c>
-      <c r="D40" t="n">
-        <v>0.138427734375</v>
-      </c>
-      <c r="E40" t="n">
-        <v>0.138427734375</v>
-      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -1125,15 +759,6 @@
       <c r="B41" t="n">
         <v>0.09375</v>
       </c>
-      <c r="C41" t="n">
-        <v>0.138427734375</v>
-      </c>
-      <c r="D41" t="n">
-        <v>0.138427734375</v>
-      </c>
-      <c r="E41" t="n">
-        <v>0.138427734375</v>
-      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -1142,15 +767,6 @@
       <c r="B42" t="n">
         <v>0.09375</v>
       </c>
-      <c r="C42" t="n">
-        <v>0.138427734375</v>
-      </c>
-      <c r="D42" t="n">
-        <v>0.138427734375</v>
-      </c>
-      <c r="E42" t="n">
-        <v>0.138427734375</v>
-      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -1159,15 +775,6 @@
       <c r="B43" t="n">
         <v>0.09375</v>
       </c>
-      <c r="C43" t="n">
-        <v>0.138427734375</v>
-      </c>
-      <c r="D43" t="n">
-        <v>0.138427734375</v>
-      </c>
-      <c r="E43" t="n">
-        <v>0.138427734375</v>
-      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -1176,15 +783,6 @@
       <c r="B44" t="n">
         <v>0.09375</v>
       </c>
-      <c r="C44" t="n">
-        <v>0.138427734375</v>
-      </c>
-      <c r="D44" t="n">
-        <v>0.138427734375</v>
-      </c>
-      <c r="E44" t="n">
-        <v>0.138427734375</v>
-      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -1193,15 +791,6 @@
       <c r="B45" t="n">
         <v>0.09375</v>
       </c>
-      <c r="C45" t="n">
-        <v>0.138427734375</v>
-      </c>
-      <c r="D45" t="n">
-        <v>0.138427734375</v>
-      </c>
-      <c r="E45" t="n">
-        <v>0.138427734375</v>
-      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -1210,15 +799,6 @@
       <c r="B46" t="n">
         <v>0.09375</v>
       </c>
-      <c r="C46" t="n">
-        <v>0.1383056640625</v>
-      </c>
-      <c r="D46" t="n">
-        <v>0.1383056640625</v>
-      </c>
-      <c r="E46" t="n">
-        <v>0.1383056640625</v>
-      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -1227,15 +807,6 @@
       <c r="B47" t="n">
         <v>0.1875</v>
       </c>
-      <c r="C47" t="n">
-        <v>0.263916015625</v>
-      </c>
-      <c r="D47" t="n">
-        <v>0.263916015625</v>
-      </c>
-      <c r="E47" t="n">
-        <v>0.263916015625</v>
-      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -1244,15 +815,6 @@
       <c r="B48" t="n">
         <v>0.1875</v>
       </c>
-      <c r="C48" t="n">
-        <v>0.263916015625</v>
-      </c>
-      <c r="D48" t="n">
-        <v>0.263916015625</v>
-      </c>
-      <c r="E48" t="n">
-        <v>0.263916015625</v>
-      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -1261,15 +823,6 @@
       <c r="B49" t="n">
         <v>0.1875</v>
       </c>
-      <c r="C49" t="n">
-        <v>0.2637939453125</v>
-      </c>
-      <c r="D49" t="n">
-        <v>0.2637939453125</v>
-      </c>
-      <c r="E49" t="n">
-        <v>0.2637939453125</v>
-      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -1278,15 +831,6 @@
       <c r="B50" t="n">
         <v>0.1875</v>
       </c>
-      <c r="C50" t="n">
-        <v>0.2637939453125</v>
-      </c>
-      <c r="D50" t="n">
-        <v>0.2637939453125</v>
-      </c>
-      <c r="E50" t="n">
-        <v>0.2637939453125</v>
-      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -1295,15 +839,6 @@
       <c r="B51" t="n">
         <v>0.1875</v>
       </c>
-      <c r="C51" t="n">
-        <v>0.2637939453125</v>
-      </c>
-      <c r="D51" t="n">
-        <v>0.2637939453125</v>
-      </c>
-      <c r="E51" t="n">
-        <v>0.2637939453125</v>
-      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -1312,15 +847,6 @@
       <c r="B52" t="n">
         <v>0.1875</v>
       </c>
-      <c r="C52" t="n">
-        <v>0.263916015625</v>
-      </c>
-      <c r="D52" t="n">
-        <v>0.263916015625</v>
-      </c>
-      <c r="E52" t="n">
-        <v>0.263916015625</v>
-      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -1329,15 +855,6 @@
       <c r="B53" t="n">
         <v>0.1875</v>
       </c>
-      <c r="C53" t="n">
-        <v>0.2640380859375</v>
-      </c>
-      <c r="D53" t="n">
-        <v>0.2640380859375</v>
-      </c>
-      <c r="E53" t="n">
-        <v>0.2640380859375</v>
-      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -1346,15 +863,6 @@
       <c r="B54" t="n">
         <v>0.1875</v>
       </c>
-      <c r="C54" t="n">
-        <v>0.2637939453125</v>
-      </c>
-      <c r="D54" t="n">
-        <v>0.2637939453125</v>
-      </c>
-      <c r="E54" t="n">
-        <v>0.2637939453125</v>
-      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -1363,15 +871,6 @@
       <c r="B55" t="n">
         <v>0.1875</v>
       </c>
-      <c r="C55" t="n">
-        <v>0.2637939453125</v>
-      </c>
-      <c r="D55" t="n">
-        <v>0.2637939453125</v>
-      </c>
-      <c r="E55" t="n">
-        <v>0.2637939453125</v>
-      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -1380,15 +879,6 @@
       <c r="B56" t="n">
         <v>0.125</v>
       </c>
-      <c r="C56" t="n">
-        <v>0.505859375</v>
-      </c>
-      <c r="D56" t="n">
-        <v>0.505859375</v>
-      </c>
-      <c r="E56" t="n">
-        <v>0.505859375</v>
-      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -1397,15 +887,6 @@
       <c r="B57" t="n">
         <v>0.125</v>
       </c>
-      <c r="C57" t="n">
-        <v>0.505859375</v>
-      </c>
-      <c r="D57" t="n">
-        <v>0.505859375</v>
-      </c>
-      <c r="E57" t="n">
-        <v>0.505859375</v>
-      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -1414,15 +895,6 @@
       <c r="B58" t="n">
         <v>0.125</v>
       </c>
-      <c r="C58" t="n">
-        <v>0.505859375</v>
-      </c>
-      <c r="D58" t="n">
-        <v>0.505859375</v>
-      </c>
-      <c r="E58" t="n">
-        <v>0.505859375</v>
-      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -1431,15 +903,6 @@
       <c r="B59" t="n">
         <v>0.125</v>
       </c>
-      <c r="C59" t="n">
-        <v>0.5059814453125</v>
-      </c>
-      <c r="D59" t="n">
-        <v>0.5059814453125</v>
-      </c>
-      <c r="E59" t="n">
-        <v>0.5059814453125</v>
-      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -1448,15 +911,6 @@
       <c r="B60" t="n">
         <v>0.125</v>
       </c>
-      <c r="C60" t="n">
-        <v>0.5059814453125</v>
-      </c>
-      <c r="D60" t="n">
-        <v>0.5059814453125</v>
-      </c>
-      <c r="E60" t="n">
-        <v>0.5059814453125</v>
-      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -1465,15 +919,6 @@
       <c r="B61" t="n">
         <v>0.125</v>
       </c>
-      <c r="C61" t="n">
-        <v>0.505859375</v>
-      </c>
-      <c r="D61" t="n">
-        <v>0.505859375</v>
-      </c>
-      <c r="E61" t="n">
-        <v>0.505859375</v>
-      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -1482,15 +927,6 @@
       <c r="B62" t="n">
         <v>0.125</v>
       </c>
-      <c r="C62" t="n">
-        <v>0.505859375</v>
-      </c>
-      <c r="D62" t="n">
-        <v>0.505859375</v>
-      </c>
-      <c r="E62" t="n">
-        <v>0.505859375</v>
-      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -1499,15 +935,6 @@
       <c r="B63" t="n">
         <v>0.125</v>
       </c>
-      <c r="C63" t="n">
-        <v>0.505859375</v>
-      </c>
-      <c r="D63" t="n">
-        <v>0.505859375</v>
-      </c>
-      <c r="E63" t="n">
-        <v>0.505859375</v>
-      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -1516,15 +943,6 @@
       <c r="B64" t="n">
         <v>0.125</v>
       </c>
-      <c r="C64" t="n">
-        <v>0.505859375</v>
-      </c>
-      <c r="D64" t="n">
-        <v>0.505859375</v>
-      </c>
-      <c r="E64" t="n">
-        <v>0.505859375</v>
-      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -1533,15 +951,6 @@
       <c r="B65" t="n">
         <v>0.125</v>
       </c>
-      <c r="C65" t="n">
-        <v>0.5059814453125</v>
-      </c>
-      <c r="D65" t="n">
-        <v>0.5059814453125</v>
-      </c>
-      <c r="E65" t="n">
-        <v>0.5059814453125</v>
-      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -1549,15 +958,6 @@
       </c>
       <c r="B66" t="n">
         <v>0.25</v>
-      </c>
-      <c r="C66" t="n">
-        <v>0.9388427734375</v>
-      </c>
-      <c r="D66" t="n">
-        <v>0.9388427734375</v>
-      </c>
-      <c r="E66" t="n">
-        <v>0.9388427734375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>